<commit_message>
Added keep_base_year_affected_obs function to keep columns affected by base year
</commit_message>
<xml_diff>
--- a/gdp_revisions_datasets/base_year_df.xlsx
+++ b/gdp_revisions_datasets/base_year_df.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/Research Assistant/CIUP/GDP Revisions/GitHub/peru_gdp_revisions/gdp_revisions_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_497511A4C457DCDFE54878D6425DCE3A06D5682C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D670663-0292-46A2-B33C-E6EED6FAFBE0}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_497511A4C457DCDFE54878D6425DCE3A06D5682C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67F70BEE-7016-49B8-93C7-94C64ABE921B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1452,7 +1452,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1508,7 +1508,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1813,13 +1813,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:OA1475"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="CD325" workbookViewId="0">
+      <selection activeCell="CN335" sqref="CM335:CN338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="9.21875" customWidth="1"/>
+    <col min="87" max="87" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:391" x14ac:dyDescent="0.3">

</xml_diff>